<commit_message>
Added high iterations report TODO: display and excel for high iterations report
</commit_message>
<xml_diff>
--- a/triager/report/report.xlsx
+++ b/triager/report/report.xlsx
@@ -407,102 +407,111 @@
     <t>Resource_SC</t>
   </si>
   <si>
+    <t>5377-12389221</t>
+  </si>
+  <si>
+    <t>Resource_VBG</t>
+  </si>
+  <si>
+    <t>Resource_SS</t>
+  </si>
+  <si>
+    <t>5377-13366202</t>
+  </si>
+  <si>
+    <t>CIU</t>
+  </si>
+  <si>
+    <t>5377-13305722</t>
+  </si>
+  <si>
+    <t>Resource_SR</t>
+  </si>
+  <si>
+    <t>5377-13095530</t>
+  </si>
+  <si>
+    <t>5377-13340424</t>
+  </si>
+  <si>
+    <t>MLOC</t>
+  </si>
+  <si>
+    <t>Resource_LH</t>
+  </si>
+  <si>
+    <t>5377-12389282</t>
+  </si>
+  <si>
+    <t>Resource_AR</t>
+  </si>
+  <si>
+    <t>5377-13341186</t>
+  </si>
+  <si>
+    <t>5377-13284729</t>
+  </si>
+  <si>
+    <t>SGCI</t>
+  </si>
+  <si>
+    <t>Resource_AK</t>
+  </si>
+  <si>
+    <t>5377-13341325</t>
+  </si>
+  <si>
+    <t>RJR</t>
+  </si>
+  <si>
+    <t>5377-13301656</t>
+  </si>
+  <si>
+    <t>Resource_AJ</t>
+  </si>
+  <si>
+    <t>5377-13341378</t>
+  </si>
+  <si>
+    <t>5377-13265067</t>
+  </si>
+  <si>
+    <t>MSM</t>
+  </si>
+  <si>
+    <t>Resource_SRB</t>
+  </si>
+  <si>
+    <t>5377-13331793</t>
+  </si>
+  <si>
+    <t>5377-13327560</t>
+  </si>
+  <si>
+    <t>Resource_SVK</t>
+  </si>
+  <si>
+    <t>5377-13311630</t>
+  </si>
+  <si>
+    <t>5377-13340578</t>
+  </si>
+  <si>
+    <t>VFS</t>
+  </si>
+  <si>
+    <t>Resource_BW</t>
+  </si>
+  <si>
     <t>5377-12626199</t>
   </si>
   <si>
-    <t>Resource_SS</t>
-  </si>
-  <si>
-    <t>5377-13366202</t>
-  </si>
-  <si>
-    <t>CIU</t>
-  </si>
-  <si>
-    <t>5377-13305722</t>
-  </si>
-  <si>
-    <t>Resource_SR</t>
-  </si>
-  <si>
-    <t>5377-13095530</t>
-  </si>
-  <si>
-    <t>5377-13340424</t>
-  </si>
-  <si>
-    <t>MLOC</t>
-  </si>
-  <si>
-    <t>Resource_LH</t>
-  </si>
-  <si>
-    <t>Resource_AR</t>
-  </si>
-  <si>
-    <t>5377-13341186</t>
-  </si>
-  <si>
-    <t>5377-13284729</t>
-  </si>
-  <si>
-    <t>SGCI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assigned directly to employee. </t>
-  </si>
-  <si>
-    <t>Resource_AK</t>
-  </si>
-  <si>
-    <t>5377-13341325</t>
-  </si>
-  <si>
-    <t>RJR</t>
-  </si>
-  <si>
-    <t>5377-13301656</t>
-  </si>
-  <si>
-    <t>Resource_AJ</t>
-  </si>
-  <si>
-    <t>5377-13341378</t>
-  </si>
-  <si>
-    <t>5377-13265067</t>
-  </si>
-  <si>
-    <t>MSM</t>
-  </si>
-  <si>
-    <t>Resource_SRB</t>
-  </si>
-  <si>
-    <t>5377-13331793</t>
-  </si>
-  <si>
-    <t>5377-13327560</t>
-  </si>
-  <si>
-    <t>Resource_SVK</t>
-  </si>
-  <si>
-    <t>5377-13311630</t>
-  </si>
-  <si>
-    <t>5377-13340578</t>
-  </si>
-  <si>
-    <t>VFS</t>
-  </si>
-  <si>
-    <t>Resource_BW</t>
-  </si>
-  <si>
     <t>5377-13255215</t>
   </si>
   <si>
+    <t>Total 4 tickets</t>
+  </si>
+  <si>
     <t>Resource_PRG</t>
   </si>
   <si>
@@ -573,15 +582,6 @@
   </si>
   <si>
     <t xml:space="preserve">Skill: Logistics. Assigned using default scheduler model. </t>
-  </si>
-  <si>
-    <t>5377-12389221</t>
-  </si>
-  <si>
-    <t>Resource_VBG</t>
-  </si>
-  <si>
-    <t>5377-12389282</t>
   </si>
   <si>
     <t>Resource_RKM</t>
@@ -2199,12 +2199,14 @@
         <v>43</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H52" s="3" t="s"/>
+      <c r="H52" s="3" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="5" t="s">
@@ -2213,13 +2215,13 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>12</v>
@@ -2232,12 +2234,12 @@
         <v>112</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="B55" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>78</v>
@@ -2263,10 +2265,10 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>114</v>
@@ -2289,10 +2291,10 @@
     </row>
     <row r="58" spans="1:8">
       <c r="B58" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>12</v>
@@ -2307,299 +2309,312 @@
         <v>30</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="5" t="s">
-        <v>34</v>
+      <c r="B59" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C60" s="3" t="s">
+      <c r="A60" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="D61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="3" t="s"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="B61" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>47</v>
       </c>
       <c r="G61" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H61" s="3" t="s"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="B62" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H61" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="5" t="s">
+      <c r="C62" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B63" s="3" t="s">
+    <row r="64" spans="1:8">
+      <c r="A64" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="C64" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F63" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H63" s="3" t="s"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="B64" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D64" s="3" t="s">
+      <c r="F64" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H64" s="3" t="s"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="B65" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H64" s="3" t="s"/>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="5" t="s">
+      <c r="F65" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H65" s="3" t="s"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B66" s="3" t="s">
+    <row r="67" spans="1:8">
+      <c r="A67" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H66" s="3" t="s"/>
-    </row>
-    <row r="67" spans="1:8">
       <c r="B67" s="3" t="s">
         <v>151</v>
       </c>
       <c r="C67" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H67" s="3" t="s"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="B68" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="C68" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H67" s="3" t="s"/>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="5" t="s">
+      <c r="F68" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H68" s="3" t="s"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B69" s="3" t="s">
+    <row r="70" spans="1:8">
+      <c r="A70" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H69" s="3" t="s"/>
-    </row>
-    <row r="70" spans="1:8">
       <c r="B70" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H70" s="3" t="s"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="B71" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="D71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="F71" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G70" s="4" t="s">
+      <c r="G71" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H70" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="5" t="s">
+      <c r="H71" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B72" s="3" t="s">
+    <row r="73" spans="1:8">
+      <c r="A73" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
       <c r="B73" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>159</v>
+        <v>49</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>160</v>
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="B74" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D74" s="3" t="s">
+    </row>
+    <row r="75" spans="1:8">
+      <c r="B75" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F75" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H75" s="3" t="s"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="B76" s="3" t="s">
         <v>163</v>
       </c>
@@ -2607,231 +2622,233 @@
         <v>76</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E76" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="F78" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G76" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="3" t="s">
+      <c r="G78" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H78" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
-      <c r="B77" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C77" s="3" t="s">
+    <row r="79" spans="1:8">
+      <c r="B79" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D79" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E79" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F77" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H77" s="3" t="s"/>
-    </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="5" t="s">
+      <c r="F79" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H79" s="3" t="s"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="3" t="s">
+    <row r="81" spans="1:8">
+      <c r="A81" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="F81" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G79" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H79" s="3" t="s">
+      <c r="G81" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H81" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
-      <c r="B80" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D80" s="3" t="s">
+    <row r="82" spans="1:8">
+      <c r="B82" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H80" s="3" t="s"/>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="H82" s="3" t="s"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="3" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="83" spans="1:8">
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H83" s="3" t="s"/>
-    </row>
-    <row r="84" spans="1:8">
-      <c r="B84" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="D84" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H84" s="3" t="s"/>
+      <c r="H84" s="3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="B85" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H85" s="3" t="s"/>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="B86" s="3" t="s">
         <v>178</v>
       </c>
       <c r="C86" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H86" s="3" t="s"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E86" s="3" t="s">
+      <c r="D88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E88" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F86" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G86" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H86" s="3" t="s"/>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="B87" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C87" s="3" t="s">
+      <c r="F88" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H88" s="3" t="s"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="B89" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H87" s="3" t="s"/>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>13</v>
@@ -2840,56 +2857,43 @@
         <v>43</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>182</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H89" s="3" t="s"/>
     </row>
     <row r="90" spans="1:8">
-      <c r="B90" s="3" t="s">
+      <c r="A90" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G90" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H90" s="3" t="s"/>
-    </row>
-    <row r="91" spans="1:8">
       <c r="B91" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>167</v>
+        <v>114</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="G91" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H91" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="H91" s="3" t="s"/>
     </row>
     <row r="92" spans="1:8">
       <c r="B92" s="3" t="s">
@@ -2899,47 +2903,43 @@
         <v>114</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H92" s="3" t="s">
-        <v>187</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="H92" s="3" t="s"/>
     </row>
     <row r="93" spans="1:8">
       <c r="B93" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G93" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G93" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H93" s="3" t="s">
-        <v>187</v>
-      </c>
+      <c r="H93" s="3" t="s"/>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" s="5" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3088,7 +3088,7 @@
         <v>30</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3277,7 +3277,7 @@
         <v>220</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>12</v>
@@ -3443,27 +3443,27 @@
     <mergeCell ref="A53:H53"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="A56:H56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:H65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A68:H68"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A71:H71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A75:H75"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A78:H78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:H81"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A85:H85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A88:H88"/>
-    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A63:H63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:H69"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A72:H72"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="A77:H77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:H83"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A87:H87"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A90:H90"/>
+    <mergeCell ref="A91:A93"/>
     <mergeCell ref="A94:H94"/>
     <mergeCell ref="A95:A96"/>
     <mergeCell ref="A97:H97"/>

</xml_diff>

<commit_message>
Added high iterations report
</commit_message>
<xml_diff>
--- a/triager/report/report.xlsx
+++ b/triager/report/report.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Triage Summary" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Allocation Recommendation" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="High Iterations" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="255">
   <si>
     <t>Triage Summary Date</t>
   </si>
@@ -65,7 +66,7 @@
     <t>B2Bi</t>
   </si>
   <si>
-    <t>18/08/2017</t>
+    <t>20/08/2017</t>
   </si>
   <si>
     <t>Resource Name</t>
@@ -705,6 +706,82 @@
   </si>
   <si>
     <t>5377-12097487</t>
+  </si>
+  <si>
+    <t>Ticket_Number</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Additional Info 1</t>
+  </si>
+  <si>
+    <t>Additional Info 2</t>
+  </si>
+  <si>
+    <t>NOV/C1(6)R1(.l5) DEC/C5(13) JAN/C1(1)M1(1) FEB/A1(1)C2(3) MAR/F1(1)M1(1)
+APR/C3(6)</t>
+  </si>
+  <si>
+    <t>MAR/Q1(1)</t>
+  </si>
+  <si>
+    <t>MAR/N JUN/C1(1.5) JUL/C1(1) AUG/C3(10.5) OCT/C1(2) NOV/R1(1.5)C2(2.5)X1(1) DEC/C2(3.5) JAN/C9(20.5)R1(.5) FEB/C4(9)F1(2)R3(5) MAR/C2(3.5) APR/C2(4)R1(0.5)</t>
+  </si>
+  <si>
+    <t>NOV/Q1 FEB/Q1</t>
+  </si>
+  <si>
+    <t>APR/C2(3.5)A3(3.2)</t>
+  </si>
+  <si>
+    <t>DEC/NA2(1.5)C3(5)M4(2.2)R1(2) JAN/R2(2.5)A2(1)C4(7)M1(.6) FEB/R1(1)C5(6.5)M1(.5) MAR/M2(1)A1(.5)C1(1) APR/M1(1)A3(1.1)C2(2.5)M1(1)</t>
+  </si>
+  <si>
+    <t>JUN/NM1(1.75)F2(2)C6(10) JUL/R1(2)C5(5.5) NOV/C1(2)</t>
+  </si>
+  <si>
+    <t>JUN/Q2</t>
+  </si>
+  <si>
+    <t>DEC/C1(3.5) JAN/C1(2)R1(1) FEB/R1(1)M3(3)A1(1)C1(2) MAR/C1(2.5)F1(1.5) APR/C1(1)</t>
+  </si>
+  <si>
+    <t>MAR/Q1</t>
+  </si>
+  <si>
+    <t>APR/NC3(8.5)</t>
+  </si>
+  <si>
+    <t>APR/C1(3.5)</t>
+  </si>
+  <si>
+    <t>APR/R2(5.5)</t>
+  </si>
+  <si>
+    <t>MAR/R2(2.5)N APR/C4(10)</t>
+  </si>
+  <si>
+    <t>DEC/NR2(3.5)C6(14.5) JAN/C5(8.5) FEB/C4(8.5)X1(1) MAR/C4(9.5)X1(.8) APR/M1(.8)C1(2)</t>
+  </si>
+  <si>
+    <t>FEB/Q1 MAR/Q1</t>
+  </si>
+  <si>
+    <t>NOV/N FEB/C1(3) NOV/R2(1)C2(6)M1(1) DEC/C1(5) JAN/C1(5) MAR/C2(4) APR/F1(4)</t>
+  </si>
+  <si>
+    <t>APR/Q1</t>
+  </si>
+  <si>
+    <t>DEC/NC1(3) JAN/C4(10)F2(2)R1(1)M1(3) JUN/C1(2)R1(2) DEC/C1(5) JAN/C1(1.5) APR/C1(2)F1(1.5)</t>
+  </si>
+  <si>
+    <t>JAN/Q2 APR/Q1</t>
+  </si>
+  <si>
+    <t>APR/R2(2.5)NC3(6)</t>
   </si>
 </sst>
 </file>
@@ -3484,4 +3561,363 @@
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="16"/>
+    <col customWidth="1" max="2" min="2" width="16"/>
+    <col customWidth="1" max="3" min="3" width="16"/>
+    <col customWidth="1" max="4" min="4" width="16"/>
+    <col customWidth="1" max="5" min="5" width="16"/>
+    <col customWidth="1" max="6" min="6" width="85"/>
+    <col customWidth="1" max="7" min="7" width="30"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="20" r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="3" spans="1:7">
+      <c r="A3" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" s="4" t="s"/>
+    </row>
+    <row customHeight="1" ht="40" r="5" spans="1:7">
+      <c r="A5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" s="4" t="s"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G8" s="4" t="s"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G9" s="4" t="s"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="4" t="s"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G11" s="4" t="s"/>
+    </row>
+    <row customHeight="1" ht="40" r="12" spans="1:7">
+      <c r="A12" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="14" spans="1:7">
+      <c r="A14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G15" s="4" t="s"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added neural net debugging report
</commit_message>
<xml_diff>
--- a/triager/report/report.xlsx
+++ b/triager/report/report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Triage Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Allocation Recommendation" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="High Iterations" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Triage Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Allocation Recommendation" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="High Iterations" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>